<commit_message>
Fix issue with SFDC Lightning
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mminarik/Documents/GitHub/arse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D831C01B-921E-6C4C-BA7A-0E5812A02EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D669C323-02DB-F744-97A9-585A0241DF3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37080" yWindow="18780" windowWidth="28040" windowHeight="17440" xr2:uid="{045089A8-F685-0C40-B1DA-0F2DC526CB3E}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added support for non-mandatory fields
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mminarik/Documents/GitHub/arse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mminarik/Documents/Python/arse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D669C323-02DB-F744-97A9-585A0241DF3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796740D2-38F9-4F47-A171-518A336E4A67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37080" yWindow="18780" windowWidth="28040" windowHeight="17440" xr2:uid="{045089A8-F685-0C40-B1DA-0F2DC526CB3E}"/>
+    <workbookView xWindow="6700" yWindow="13500" windowWidth="28040" windowHeight="17440" xr2:uid="{045089A8-F685-0C40-B1DA-0F2DC526CB3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>date</t>
   </si>
@@ -82,6 +82,36 @@
   </si>
   <si>
     <t>Meetings</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>This is something.</t>
+  </si>
+  <si>
+    <t>next_step</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>EUC</t>
+  </si>
+  <si>
+    <t>solution</t>
+  </si>
+  <si>
+    <t>HORIZON ON PREM</t>
+  </si>
+  <si>
+    <t>HORIZON STD</t>
+  </si>
+  <si>
+    <t>activity_category</t>
+  </si>
+  <si>
+    <t>solution_product</t>
   </si>
 </sst>
 </file>
@@ -434,20 +464,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B186DADD-3286-C74C-8F5B-8480E2874F87}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,19 +494,34 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44166</v>
       </c>
@@ -486,14 +534,17 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44166</v>
       </c>
@@ -506,16 +557,31 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>